<commit_message>
Add new Menking data
</commit_message>
<xml_diff>
--- a/data/raw/menking-et-al-2025/spline-fits-for-ZN_CMIP7.xlsx
+++ b/data/raw/menking-et-al-2025/spline-fits-for-ZN_CMIP7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/men111_csiro_au/Documents/Documents/James Menking/Documents/geology/coding and modeling/CMIP7/data for ZN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{B72F3D14-A108-41D2-8591-D1EB2B7A6A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C55E3A95-99A4-46D5-BDDD-2BD218F187D0}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{B72F3D14-A108-41D2-8591-D1EB2B7A6A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B733DDA9-1076-4717-AAEE-06C6B0167A68}"/>
   <bookViews>
-    <workbookView xWindow="-39405" yWindow="-4755" windowWidth="34020" windowHeight="19140" xr2:uid="{C592550F-3943-4119-BF5B-1E2CB536A048}"/>
+    <workbookView xWindow="-50910" yWindow="-5130" windowWidth="19920" windowHeight="20580" xr2:uid="{C592550F-3943-4119-BF5B-1E2CB536A048}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,11 +101,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -121,6 +122,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -442,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFAA6A3-7DBD-4979-9841-908F6AB38E31}">
   <dimension ref="A1:E2032"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+    <sheetView tabSelected="1" topLeftCell="A1983" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26194,11 +26199,11 @@
       <c r="B1843">
         <v>284.06</v>
       </c>
-      <c r="D1843">
+      <c r="D1843" s="2">
         <v>1840</v>
       </c>
-      <c r="E1843">
-        <v>270.44</v>
+      <c r="E1843" s="2">
+        <v>270.37</v>
       </c>
     </row>
     <row r="1844" spans="1:5" x14ac:dyDescent="0.25">
@@ -26208,11 +26213,11 @@
       <c r="B1844">
         <v>284.02999999999997</v>
       </c>
-      <c r="D1844">
+      <c r="D1844" s="2">
         <v>1841</v>
       </c>
-      <c r="E1844">
-        <v>270.51</v>
+      <c r="E1844" s="2">
+        <v>270.48</v>
       </c>
     </row>
     <row r="1845" spans="1:5" x14ac:dyDescent="0.25">
@@ -26222,11 +26227,11 @@
       <c r="B1845">
         <v>284.01</v>
       </c>
-      <c r="D1845">
+      <c r="D1845" s="2">
         <v>1842</v>
       </c>
-      <c r="E1845">
-        <v>270.58</v>
+      <c r="E1845" s="2">
+        <v>270.60000000000002</v>
       </c>
     </row>
     <row r="1846" spans="1:5" x14ac:dyDescent="0.25">
@@ -26236,11 +26241,11 @@
       <c r="B1846">
         <v>283.99</v>
       </c>
-      <c r="D1846">
+      <c r="D1846" s="2">
         <v>1843</v>
       </c>
-      <c r="E1846">
-        <v>270.66000000000003</v>
+      <c r="E1846" s="2">
+        <v>270.72000000000003</v>
       </c>
     </row>
     <row r="1847" spans="1:5" x14ac:dyDescent="0.25">
@@ -26250,11 +26255,11 @@
       <c r="B1847">
         <v>283.99</v>
       </c>
-      <c r="D1847">
+      <c r="D1847" s="2">
         <v>1844</v>
       </c>
-      <c r="E1847">
-        <v>270.73</v>
+      <c r="E1847" s="2">
+        <v>270.83999999999997</v>
       </c>
     </row>
     <row r="1848" spans="1:5" x14ac:dyDescent="0.25">
@@ -26264,11 +26269,11 @@
       <c r="B1848">
         <v>284.01</v>
       </c>
-      <c r="D1848">
+      <c r="D1848" s="2">
         <v>1845</v>
       </c>
-      <c r="E1848">
-        <v>270.81</v>
+      <c r="E1848" s="2">
+        <v>270.97000000000003</v>
       </c>
     </row>
     <row r="1849" spans="1:5" x14ac:dyDescent="0.25">
@@ -26278,11 +26283,11 @@
       <c r="B1849">
         <v>284.04000000000002</v>
       </c>
-      <c r="D1849">
+      <c r="D1849" s="2">
         <v>1846</v>
       </c>
-      <c r="E1849">
-        <v>270.89</v>
+      <c r="E1849" s="2">
+        <v>271.08999999999997</v>
       </c>
     </row>
     <row r="1850" spans="1:5" x14ac:dyDescent="0.25">
@@ -26292,11 +26297,11 @@
       <c r="B1850">
         <v>284.08999999999997</v>
       </c>
-      <c r="D1850">
+      <c r="D1850" s="2">
         <v>1847</v>
       </c>
-      <c r="E1850">
-        <v>270.97000000000003</v>
+      <c r="E1850" s="2">
+        <v>271.20999999999998</v>
       </c>
     </row>
     <row r="1851" spans="1:5" x14ac:dyDescent="0.25">
@@ -26306,11 +26311,11 @@
       <c r="B1851">
         <v>284.16000000000003</v>
       </c>
-      <c r="D1851">
+      <c r="D1851" s="2">
         <v>1848</v>
       </c>
-      <c r="E1851">
-        <v>271.05</v>
+      <c r="E1851" s="2">
+        <v>271.33</v>
       </c>
     </row>
     <row r="1852" spans="1:5" x14ac:dyDescent="0.25">
@@ -26320,11 +26325,11 @@
       <c r="B1852">
         <v>284.26</v>
       </c>
-      <c r="D1852">
+      <c r="D1852" s="2">
         <v>1849</v>
       </c>
-      <c r="E1852">
-        <v>271.13</v>
+      <c r="E1852" s="2">
+        <v>271.45</v>
       </c>
     </row>
     <row r="1853" spans="1:5" x14ac:dyDescent="0.25">
@@ -26334,11 +26339,11 @@
       <c r="B1853">
         <v>284.37</v>
       </c>
-      <c r="D1853">
-        <v>1851</v>
-      </c>
-      <c r="E1853">
-        <v>271.35000000000002</v>
+      <c r="D1853" s="2">
+        <v>1850</v>
+      </c>
+      <c r="E1853" s="2">
+        <v>271.57</v>
       </c>
     </row>
     <row r="1854" spans="1:5" x14ac:dyDescent="0.25">
@@ -26348,11 +26353,11 @@
       <c r="B1854">
         <v>284.49</v>
       </c>
-      <c r="D1854">
-        <v>1852</v>
-      </c>
-      <c r="E1854">
-        <v>271.5</v>
+      <c r="D1854" s="2">
+        <v>1851</v>
+      </c>
+      <c r="E1854" s="2">
+        <v>271.69</v>
       </c>
     </row>
     <row r="1855" spans="1:5" x14ac:dyDescent="0.25">
@@ -26362,11 +26367,11 @@
       <c r="B1855">
         <v>284.62</v>
       </c>
-      <c r="D1855">
-        <v>1853</v>
-      </c>
-      <c r="E1855">
-        <v>271.64</v>
+      <c r="D1855" s="2">
+        <v>1852</v>
+      </c>
+      <c r="E1855" s="2">
+        <v>271.82</v>
       </c>
     </row>
     <row r="1856" spans="1:5" x14ac:dyDescent="0.25">
@@ -26376,11 +26381,11 @@
       <c r="B1856">
         <v>284.75</v>
       </c>
-      <c r="D1856">
-        <v>1854</v>
-      </c>
-      <c r="E1856">
-        <v>271.77999999999997</v>
+      <c r="D1856" s="2">
+        <v>1853</v>
+      </c>
+      <c r="E1856" s="2">
+        <v>271.94</v>
       </c>
     </row>
     <row r="1857" spans="1:5" x14ac:dyDescent="0.25">
@@ -26390,11 +26395,11 @@
       <c r="B1857">
         <v>284.88</v>
       </c>
-      <c r="D1857">
-        <v>1855</v>
-      </c>
-      <c r="E1857">
-        <v>271.92</v>
+      <c r="D1857" s="2">
+        <v>1854</v>
+      </c>
+      <c r="E1857" s="2">
+        <v>272.06</v>
       </c>
     </row>
     <row r="1858" spans="1:5" x14ac:dyDescent="0.25">
@@ -26404,11 +26409,11 @@
       <c r="B1858">
         <v>285</v>
       </c>
-      <c r="D1858">
-        <v>1856</v>
-      </c>
-      <c r="E1858">
-        <v>272.07</v>
+      <c r="D1858" s="2">
+        <v>1855</v>
+      </c>
+      <c r="E1858" s="2">
+        <v>272.19</v>
       </c>
     </row>
     <row r="1859" spans="1:5" x14ac:dyDescent="0.25">
@@ -26418,11 +26423,11 @@
       <c r="B1859">
         <v>285.13</v>
       </c>
-      <c r="D1859">
-        <v>1857</v>
-      </c>
-      <c r="E1859">
-        <v>272.20999999999998</v>
+      <c r="D1859" s="2">
+        <v>1856</v>
+      </c>
+      <c r="E1859" s="2">
+        <v>272.31</v>
       </c>
     </row>
     <row r="1860" spans="1:5" x14ac:dyDescent="0.25">
@@ -26432,11 +26437,11 @@
       <c r="B1860">
         <v>285.25</v>
       </c>
-      <c r="D1860">
-        <v>1858</v>
-      </c>
-      <c r="E1860">
-        <v>272.35000000000002</v>
+      <c r="D1860" s="2">
+        <v>1857</v>
+      </c>
+      <c r="E1860" s="2">
+        <v>272.43</v>
       </c>
     </row>
     <row r="1861" spans="1:5" x14ac:dyDescent="0.25">
@@ -26446,11 +26451,11 @@
       <c r="B1861">
         <v>285.37</v>
       </c>
-      <c r="D1861">
-        <v>1859</v>
-      </c>
-      <c r="E1861">
-        <v>272.49</v>
+      <c r="D1861" s="2">
+        <v>1858</v>
+      </c>
+      <c r="E1861" s="2">
+        <v>272.56</v>
       </c>
     </row>
     <row r="1862" spans="1:5" x14ac:dyDescent="0.25">
@@ -26460,11 +26465,11 @@
       <c r="B1862">
         <v>285.48</v>
       </c>
-      <c r="D1862">
-        <v>1860</v>
-      </c>
-      <c r="E1862">
-        <v>272.62</v>
+      <c r="D1862" s="2">
+        <v>1859</v>
+      </c>
+      <c r="E1862" s="2">
+        <v>272.68</v>
       </c>
     </row>
     <row r="1863" spans="1:5" x14ac:dyDescent="0.25">
@@ -26474,11 +26479,11 @@
       <c r="B1863">
         <v>285.60000000000002</v>
       </c>
-      <c r="D1863">
-        <v>1861</v>
-      </c>
-      <c r="E1863">
-        <v>272.76</v>
+      <c r="D1863" s="2">
+        <v>1860</v>
+      </c>
+      <c r="E1863" s="2">
+        <v>272.8</v>
       </c>
     </row>
     <row r="1864" spans="1:5" x14ac:dyDescent="0.25">
@@ -26488,11 +26493,11 @@
       <c r="B1864">
         <v>285.70999999999998</v>
       </c>
-      <c r="D1864">
-        <v>1862</v>
-      </c>
-      <c r="E1864">
-        <v>272.89</v>
+      <c r="D1864" s="2">
+        <v>1861</v>
+      </c>
+      <c r="E1864" s="2">
+        <v>272.93</v>
       </c>
     </row>
     <row r="1865" spans="1:5" x14ac:dyDescent="0.25">
@@ -26502,11 +26507,11 @@
       <c r="B1865">
         <v>285.83</v>
       </c>
-      <c r="D1865">
-        <v>1863</v>
-      </c>
-      <c r="E1865">
-        <v>273.02</v>
+      <c r="D1865" s="2">
+        <v>1862</v>
+      </c>
+      <c r="E1865" s="2">
+        <v>273.04000000000002</v>
       </c>
     </row>
     <row r="1866" spans="1:5" x14ac:dyDescent="0.25">
@@ -26516,11 +26521,11 @@
       <c r="B1866">
         <v>285.95</v>
       </c>
-      <c r="D1866">
-        <v>1864</v>
-      </c>
-      <c r="E1866">
-        <v>273.14999999999998</v>
+      <c r="D1866" s="2">
+        <v>1863</v>
+      </c>
+      <c r="E1866" s="2">
+        <v>273.16000000000003</v>
       </c>
     </row>
     <row r="1867" spans="1:5" x14ac:dyDescent="0.25">
@@ -26530,10 +26535,10 @@
       <c r="B1867">
         <v>286.07</v>
       </c>
-      <c r="D1867">
-        <v>1865</v>
-      </c>
-      <c r="E1867">
+      <c r="D1867" s="2">
+        <v>1864</v>
+      </c>
+      <c r="E1867" s="2">
         <v>273.27</v>
       </c>
     </row>
@@ -26544,11 +26549,11 @@
       <c r="B1868">
         <v>286.2</v>
       </c>
-      <c r="D1868">
-        <v>1866</v>
-      </c>
-      <c r="E1868">
-        <v>273.39</v>
+      <c r="D1868" s="2">
+        <v>1865</v>
+      </c>
+      <c r="E1868" s="2">
+        <v>273.38</v>
       </c>
     </row>
     <row r="1869" spans="1:5" x14ac:dyDescent="0.25">
@@ -26558,11 +26563,11 @@
       <c r="B1869">
         <v>286.33</v>
       </c>
-      <c r="D1869">
-        <v>1867</v>
-      </c>
-      <c r="E1869">
-        <v>273.5</v>
+      <c r="D1869" s="2">
+        <v>1866</v>
+      </c>
+      <c r="E1869" s="2">
+        <v>273.49</v>
       </c>
     </row>
     <row r="1870" spans="1:5" x14ac:dyDescent="0.25">
@@ -26572,11 +26577,11 @@
       <c r="B1870">
         <v>286.45999999999998</v>
       </c>
-      <c r="D1870">
-        <v>1868</v>
-      </c>
-      <c r="E1870">
-        <v>273.62</v>
+      <c r="D1870" s="2">
+        <v>1867</v>
+      </c>
+      <c r="E1870" s="2">
+        <v>273.60000000000002</v>
       </c>
     </row>
     <row r="1871" spans="1:5" x14ac:dyDescent="0.25">
@@ -26586,11 +26591,11 @@
       <c r="B1871">
         <v>286.60000000000002</v>
       </c>
-      <c r="D1871">
-        <v>1869</v>
-      </c>
-      <c r="E1871">
-        <v>273.73</v>
+      <c r="D1871" s="2">
+        <v>1868</v>
+      </c>
+      <c r="E1871" s="2">
+        <v>273.7</v>
       </c>
     </row>
     <row r="1872" spans="1:5" x14ac:dyDescent="0.25">
@@ -26600,11 +26605,11 @@
       <c r="B1872">
         <v>286.75</v>
       </c>
-      <c r="D1872">
-        <v>1870</v>
-      </c>
-      <c r="E1872">
-        <v>273.83</v>
+      <c r="D1872" s="2">
+        <v>1869</v>
+      </c>
+      <c r="E1872" s="2">
+        <v>273.8</v>
       </c>
     </row>
     <row r="1873" spans="1:5" x14ac:dyDescent="0.25">
@@ -26614,11 +26619,11 @@
       <c r="B1873">
         <v>286.89999999999998</v>
       </c>
-      <c r="D1873">
-        <v>1871</v>
-      </c>
-      <c r="E1873">
-        <v>273.94</v>
+      <c r="D1873" s="2">
+        <v>1870</v>
+      </c>
+      <c r="E1873" s="2">
+        <v>273.89</v>
       </c>
     </row>
     <row r="1874" spans="1:5" x14ac:dyDescent="0.25">
@@ -26628,11 +26633,11 @@
       <c r="B1874">
         <v>287.06</v>
       </c>
-      <c r="D1874">
-        <v>1872</v>
-      </c>
-      <c r="E1874">
-        <v>274.05</v>
+      <c r="D1874" s="2">
+        <v>1871</v>
+      </c>
+      <c r="E1874" s="2">
+        <v>273.99</v>
       </c>
     </row>
     <row r="1875" spans="1:5" x14ac:dyDescent="0.25">
@@ -26642,11 +26647,11 @@
       <c r="B1875">
         <v>287.23</v>
       </c>
-      <c r="D1875">
-        <v>1873</v>
-      </c>
-      <c r="E1875">
-        <v>274.14999999999998</v>
+      <c r="D1875" s="2">
+        <v>1872</v>
+      </c>
+      <c r="E1875" s="2">
+        <v>274.08</v>
       </c>
     </row>
     <row r="1876" spans="1:5" x14ac:dyDescent="0.25">
@@ -26656,11 +26661,11 @@
       <c r="B1876">
         <v>287.39999999999998</v>
       </c>
-      <c r="D1876">
-        <v>1874</v>
-      </c>
-      <c r="E1876">
-        <v>274.25</v>
+      <c r="D1876" s="2">
+        <v>1873</v>
+      </c>
+      <c r="E1876" s="2">
+        <v>274.18</v>
       </c>
     </row>
     <row r="1877" spans="1:5" x14ac:dyDescent="0.25">
@@ -26670,11 +26675,11 @@
       <c r="B1877">
         <v>287.57</v>
       </c>
-      <c r="D1877">
-        <v>1875</v>
-      </c>
-      <c r="E1877">
-        <v>274.36</v>
+      <c r="D1877" s="2">
+        <v>1874</v>
+      </c>
+      <c r="E1877" s="2">
+        <v>274.27</v>
       </c>
     </row>
     <row r="1878" spans="1:5" x14ac:dyDescent="0.25">
@@ -26684,11 +26689,11 @@
       <c r="B1878">
         <v>287.75</v>
       </c>
-      <c r="D1878">
-        <v>1876</v>
-      </c>
-      <c r="E1878">
-        <v>274.47000000000003</v>
+      <c r="D1878" s="2">
+        <v>1875</v>
+      </c>
+      <c r="E1878" s="2">
+        <v>274.37</v>
       </c>
     </row>
     <row r="1879" spans="1:5" x14ac:dyDescent="0.25">
@@ -26698,11 +26703,11 @@
       <c r="B1879">
         <v>287.92</v>
       </c>
-      <c r="D1879">
-        <v>1877</v>
-      </c>
-      <c r="E1879">
-        <v>274.57</v>
+      <c r="D1879" s="2">
+        <v>1876</v>
+      </c>
+      <c r="E1879" s="2">
+        <v>274.47000000000003</v>
       </c>
     </row>
     <row r="1880" spans="1:5" x14ac:dyDescent="0.25">
@@ -26712,11 +26717,11 @@
       <c r="B1880">
         <v>288.10000000000002</v>
       </c>
-      <c r="D1880">
-        <v>1878</v>
-      </c>
-      <c r="E1880">
-        <v>274.68</v>
+      <c r="D1880" s="2">
+        <v>1877</v>
+      </c>
+      <c r="E1880" s="2">
+        <v>274.57</v>
       </c>
     </row>
     <row r="1881" spans="1:5" x14ac:dyDescent="0.25">
@@ -26726,11 +26731,11 @@
       <c r="B1881">
         <v>288.27</v>
       </c>
-      <c r="D1881">
-        <v>1879</v>
-      </c>
-      <c r="E1881">
-        <v>274.8</v>
+      <c r="D1881" s="2">
+        <v>1878</v>
+      </c>
+      <c r="E1881" s="2">
+        <v>274.67</v>
       </c>
     </row>
     <row r="1882" spans="1:5" x14ac:dyDescent="0.25">
@@ -26740,11 +26745,11 @@
       <c r="B1882">
         <v>288.44</v>
       </c>
-      <c r="D1882">
-        <v>1880</v>
-      </c>
-      <c r="E1882">
-        <v>274.91000000000003</v>
+      <c r="D1882" s="2">
+        <v>1879</v>
+      </c>
+      <c r="E1882" s="2">
+        <v>274.77999999999997</v>
       </c>
     </row>
     <row r="1883" spans="1:5" x14ac:dyDescent="0.25">
@@ -26754,11 +26759,11 @@
       <c r="B1883">
         <v>288.62</v>
       </c>
-      <c r="D1883">
-        <v>1881</v>
-      </c>
-      <c r="E1883">
-        <v>275.04000000000002</v>
+      <c r="D1883" s="2">
+        <v>1880</v>
+      </c>
+      <c r="E1883" s="2">
+        <v>274.89</v>
       </c>
     </row>
     <row r="1884" spans="1:5" x14ac:dyDescent="0.25">
@@ -26768,11 +26773,11 @@
       <c r="B1884">
         <v>288.8</v>
       </c>
-      <c r="D1884">
-        <v>1882</v>
-      </c>
-      <c r="E1884">
-        <v>275.16000000000003</v>
+      <c r="D1884" s="2">
+        <v>1881</v>
+      </c>
+      <c r="E1884" s="2">
+        <v>275</v>
       </c>
     </row>
     <row r="1885" spans="1:5" x14ac:dyDescent="0.25">
@@ -26782,11 +26787,11 @@
       <c r="B1885">
         <v>289</v>
       </c>
-      <c r="D1885">
-        <v>1883</v>
-      </c>
-      <c r="E1885">
-        <v>275.29000000000002</v>
+      <c r="D1885" s="2">
+        <v>1882</v>
+      </c>
+      <c r="E1885" s="2">
+        <v>275.13</v>
       </c>
     </row>
     <row r="1886" spans="1:5" x14ac:dyDescent="0.25">
@@ -26796,11 +26801,11 @@
       <c r="B1886">
         <v>289.20999999999998</v>
       </c>
-      <c r="D1886">
-        <v>1884</v>
-      </c>
-      <c r="E1886">
-        <v>275.43</v>
+      <c r="D1886" s="2">
+        <v>1883</v>
+      </c>
+      <c r="E1886" s="2">
+        <v>275.25</v>
       </c>
     </row>
     <row r="1887" spans="1:5" x14ac:dyDescent="0.25">
@@ -26810,11 +26815,11 @@
       <c r="B1887">
         <v>289.43</v>
       </c>
-      <c r="D1887">
-        <v>1885</v>
-      </c>
-      <c r="E1887">
-        <v>275.56</v>
+      <c r="D1887" s="2">
+        <v>1884</v>
+      </c>
+      <c r="E1887" s="2">
+        <v>275.39</v>
       </c>
     </row>
     <row r="1888" spans="1:5" x14ac:dyDescent="0.25">
@@ -26824,11 +26829,11 @@
       <c r="B1888">
         <v>289.68</v>
       </c>
-      <c r="D1888">
-        <v>1886</v>
-      </c>
-      <c r="E1888">
-        <v>275.70999999999998</v>
+      <c r="D1888" s="2">
+        <v>1885</v>
+      </c>
+      <c r="E1888" s="2">
+        <v>275.52</v>
       </c>
     </row>
     <row r="1889" spans="1:5" x14ac:dyDescent="0.25">
@@ -26838,11 +26843,11 @@
       <c r="B1889">
         <v>289.95</v>
       </c>
-      <c r="D1889">
-        <v>1887</v>
-      </c>
-      <c r="E1889">
-        <v>275.85000000000002</v>
+      <c r="D1889" s="2">
+        <v>1886</v>
+      </c>
+      <c r="E1889" s="2">
+        <v>275.66000000000003</v>
       </c>
     </row>
     <row r="1890" spans="1:5" x14ac:dyDescent="0.25">
@@ -26852,11 +26857,11 @@
       <c r="B1890">
         <v>290.23</v>
       </c>
-      <c r="D1890">
-        <v>1888</v>
-      </c>
-      <c r="E1890">
-        <v>276</v>
+      <c r="D1890" s="2">
+        <v>1887</v>
+      </c>
+      <c r="E1890" s="2">
+        <v>275.81</v>
       </c>
     </row>
     <row r="1891" spans="1:5" x14ac:dyDescent="0.25">
@@ -26866,11 +26871,11 @@
       <c r="B1891">
         <v>290.52</v>
       </c>
-      <c r="D1891">
-        <v>1889</v>
-      </c>
-      <c r="E1891">
-        <v>276.14999999999998</v>
+      <c r="D1891" s="2">
+        <v>1888</v>
+      </c>
+      <c r="E1891" s="2">
+        <v>275.95</v>
       </c>
     </row>
     <row r="1892" spans="1:5" x14ac:dyDescent="0.25">
@@ -26880,11 +26885,11 @@
       <c r="B1892">
         <v>290.82</v>
       </c>
-      <c r="D1892">
-        <v>1890</v>
-      </c>
-      <c r="E1892">
-        <v>276.31</v>
+      <c r="D1892" s="2">
+        <v>1889</v>
+      </c>
+      <c r="E1892" s="2">
+        <v>276.11</v>
       </c>
     </row>
     <row r="1893" spans="1:5" x14ac:dyDescent="0.25">
@@ -26894,11 +26899,11 @@
       <c r="B1893">
         <v>291.14</v>
       </c>
-      <c r="D1893">
-        <v>1891</v>
-      </c>
-      <c r="E1893">
-        <v>276.47000000000003</v>
+      <c r="D1893" s="2">
+        <v>1890</v>
+      </c>
+      <c r="E1893" s="2">
+        <v>276.26</v>
       </c>
     </row>
     <row r="1894" spans="1:5" x14ac:dyDescent="0.25">
@@ -26908,11 +26913,11 @@
       <c r="B1894">
         <v>291.45999999999998</v>
       </c>
-      <c r="D1894">
-        <v>1892</v>
-      </c>
-      <c r="E1894">
-        <v>276.64</v>
+      <c r="D1894" s="2">
+        <v>1891</v>
+      </c>
+      <c r="E1894" s="2">
+        <v>276.42</v>
       </c>
     </row>
     <row r="1895" spans="1:5" x14ac:dyDescent="0.25">
@@ -26922,11 +26927,11 @@
       <c r="B1895">
         <v>291.8</v>
       </c>
-      <c r="D1895">
-        <v>1893</v>
-      </c>
-      <c r="E1895">
-        <v>276.81</v>
+      <c r="D1895" s="2">
+        <v>1892</v>
+      </c>
+      <c r="E1895" s="2">
+        <v>276.58999999999997</v>
       </c>
     </row>
     <row r="1896" spans="1:5" x14ac:dyDescent="0.25">
@@ -26936,11 +26941,11 @@
       <c r="B1896">
         <v>292.14</v>
       </c>
-      <c r="D1896">
-        <v>1894</v>
-      </c>
-      <c r="E1896">
-        <v>276.99</v>
+      <c r="D1896" s="2">
+        <v>1893</v>
+      </c>
+      <c r="E1896" s="2">
+        <v>276.76</v>
       </c>
     </row>
     <row r="1897" spans="1:5" x14ac:dyDescent="0.25">
@@ -26950,11 +26955,11 @@
       <c r="B1897">
         <v>292.48</v>
       </c>
-      <c r="D1897">
-        <v>1895</v>
-      </c>
-      <c r="E1897">
-        <v>277.17</v>
+      <c r="D1897" s="2">
+        <v>1894</v>
+      </c>
+      <c r="E1897" s="2">
+        <v>276.93</v>
       </c>
     </row>
     <row r="1898" spans="1:5" x14ac:dyDescent="0.25">
@@ -26964,11 +26969,11 @@
       <c r="B1898">
         <v>292.82</v>
       </c>
-      <c r="D1898">
-        <v>1896</v>
-      </c>
-      <c r="E1898">
-        <v>277.36</v>
+      <c r="D1898" s="2">
+        <v>1895</v>
+      </c>
+      <c r="E1898" s="2">
+        <v>277.11</v>
       </c>
     </row>
     <row r="1899" spans="1:5" x14ac:dyDescent="0.25">
@@ -26978,11 +26983,11 @@
       <c r="B1899">
         <v>293.16000000000003</v>
       </c>
-      <c r="D1899">
-        <v>1897</v>
-      </c>
-      <c r="E1899">
-        <v>277.55</v>
+      <c r="D1899" s="2">
+        <v>1896</v>
+      </c>
+      <c r="E1899" s="2">
+        <v>277.3</v>
       </c>
     </row>
     <row r="1900" spans="1:5" x14ac:dyDescent="0.25">
@@ -26992,11 +26997,11 @@
       <c r="B1900">
         <v>293.5</v>
       </c>
-      <c r="D1900">
-        <v>1898</v>
-      </c>
-      <c r="E1900">
-        <v>277.75</v>
+      <c r="D1900" s="2">
+        <v>1897</v>
+      </c>
+      <c r="E1900" s="2">
+        <v>277.49</v>
       </c>
     </row>
     <row r="1901" spans="1:5" x14ac:dyDescent="0.25">
@@ -27006,11 +27011,11 @@
       <c r="B1901">
         <v>293.82</v>
       </c>
-      <c r="D1901">
-        <v>1899</v>
-      </c>
-      <c r="E1901">
-        <v>277.97000000000003</v>
+      <c r="D1901" s="2">
+        <v>1898</v>
+      </c>
+      <c r="E1901" s="2">
+        <v>277.7</v>
       </c>
     </row>
     <row r="1902" spans="1:5" x14ac:dyDescent="0.25">
@@ -27020,11 +27025,11 @@
       <c r="B1902">
         <v>294.14</v>
       </c>
-      <c r="D1902">
-        <v>1900</v>
-      </c>
-      <c r="E1902">
-        <v>278.18</v>
+      <c r="D1902" s="2">
+        <v>1899</v>
+      </c>
+      <c r="E1902" s="2">
+        <v>277.91000000000003</v>
       </c>
     </row>
     <row r="1903" spans="1:5" x14ac:dyDescent="0.25">
@@ -27034,11 +27039,11 @@
       <c r="B1903">
         <v>294.45999999999998</v>
       </c>
-      <c r="D1903">
-        <v>1901</v>
-      </c>
-      <c r="E1903">
-        <v>278.41000000000003</v>
+      <c r="D1903" s="2">
+        <v>1900</v>
+      </c>
+      <c r="E1903" s="2">
+        <v>278.13</v>
       </c>
     </row>
     <row r="1904" spans="1:5" x14ac:dyDescent="0.25">
@@ -27048,11 +27053,11 @@
       <c r="B1904">
         <v>294.77</v>
       </c>
-      <c r="D1904">
-        <v>1902</v>
-      </c>
-      <c r="E1904">
-        <v>278.64</v>
+      <c r="D1904" s="2">
+        <v>1901</v>
+      </c>
+      <c r="E1904" s="2">
+        <v>278.36</v>
       </c>
     </row>
     <row r="1905" spans="1:5" x14ac:dyDescent="0.25">
@@ -27062,11 +27067,11 @@
       <c r="B1905">
         <v>295.08</v>
       </c>
-      <c r="D1905">
-        <v>1903</v>
-      </c>
-      <c r="E1905">
-        <v>278.88</v>
+      <c r="D1905" s="2">
+        <v>1902</v>
+      </c>
+      <c r="E1905" s="2">
+        <v>278.58999999999997</v>
       </c>
     </row>
     <row r="1906" spans="1:5" x14ac:dyDescent="0.25">
@@ -27076,11 +27081,11 @@
       <c r="B1906">
         <v>295.39999999999998</v>
       </c>
-      <c r="D1906">
-        <v>1904</v>
-      </c>
-      <c r="E1906">
-        <v>279.12</v>
+      <c r="D1906" s="2">
+        <v>1903</v>
+      </c>
+      <c r="E1906" s="2">
+        <v>278.83</v>
       </c>
     </row>
     <row r="1907" spans="1:5" x14ac:dyDescent="0.25">
@@ -27090,11 +27095,11 @@
       <c r="B1907">
         <v>295.72000000000003</v>
       </c>
-      <c r="D1907">
-        <v>1905</v>
-      </c>
-      <c r="E1907">
-        <v>279.37</v>
+      <c r="D1907" s="2">
+        <v>1904</v>
+      </c>
+      <c r="E1907" s="2">
+        <v>279.08</v>
       </c>
     </row>
     <row r="1908" spans="1:5" x14ac:dyDescent="0.25">
@@ -27104,11 +27109,11 @@
       <c r="B1908">
         <v>296.04000000000002</v>
       </c>
-      <c r="D1908">
-        <v>1906</v>
-      </c>
-      <c r="E1908">
-        <v>279.62</v>
+      <c r="D1908" s="2">
+        <v>1905</v>
+      </c>
+      <c r="E1908" s="2">
+        <v>279.33</v>
       </c>
     </row>
     <row r="1909" spans="1:5" x14ac:dyDescent="0.25">
@@ -27118,11 +27123,11 @@
       <c r="B1909">
         <v>296.36</v>
       </c>
-      <c r="D1909">
-        <v>1907</v>
-      </c>
-      <c r="E1909">
-        <v>279.88</v>
+      <c r="D1909" s="2">
+        <v>1906</v>
+      </c>
+      <c r="E1909" s="2">
+        <v>279.58999999999997</v>
       </c>
     </row>
     <row r="1910" spans="1:5" x14ac:dyDescent="0.25">
@@ -27132,11 +27137,11 @@
       <c r="B1910">
         <v>296.68</v>
       </c>
-      <c r="D1910">
-        <v>1908</v>
-      </c>
-      <c r="E1910">
-        <v>280.14</v>
+      <c r="D1910" s="2">
+        <v>1907</v>
+      </c>
+      <c r="E1910" s="2">
+        <v>279.85000000000002</v>
       </c>
     </row>
     <row r="1911" spans="1:5" x14ac:dyDescent="0.25">
@@ -27146,11 +27151,11 @@
       <c r="B1911">
         <v>297</v>
       </c>
-      <c r="D1911">
-        <v>1909</v>
-      </c>
-      <c r="E1911">
-        <v>280.41000000000003</v>
+      <c r="D1911" s="2">
+        <v>1908</v>
+      </c>
+      <c r="E1911" s="2">
+        <v>280.12</v>
       </c>
     </row>
     <row r="1912" spans="1:5" x14ac:dyDescent="0.25">
@@ -27160,11 +27165,11 @@
       <c r="B1912">
         <v>297.32</v>
       </c>
-      <c r="D1912">
-        <v>1910</v>
-      </c>
-      <c r="E1912">
-        <v>280.68</v>
+      <c r="D1912" s="2">
+        <v>1909</v>
+      </c>
+      <c r="E1912" s="2">
+        <v>280.39</v>
       </c>
     </row>
     <row r="1913" spans="1:5" x14ac:dyDescent="0.25">
@@ -27174,11 +27179,11 @@
       <c r="B1913">
         <v>297.64</v>
       </c>
-      <c r="D1913">
-        <v>1911</v>
-      </c>
-      <c r="E1913">
-        <v>280.95</v>
+      <c r="D1913" s="2">
+        <v>1910</v>
+      </c>
+      <c r="E1913" s="2">
+        <v>280.66000000000003</v>
       </c>
     </row>
     <row r="1914" spans="1:5" x14ac:dyDescent="0.25">
@@ -27188,11 +27193,11 @@
       <c r="B1914">
         <v>297.95</v>
       </c>
-      <c r="D1914">
-        <v>1912</v>
-      </c>
-      <c r="E1914">
-        <v>281.22000000000003</v>
+      <c r="D1914" s="2">
+        <v>1911</v>
+      </c>
+      <c r="E1914" s="2">
+        <v>280.94</v>
       </c>
     </row>
     <row r="1915" spans="1:5" x14ac:dyDescent="0.25">
@@ -27202,11 +27207,11 @@
       <c r="B1915">
         <v>298.26</v>
       </c>
-      <c r="D1915">
-        <v>1913</v>
-      </c>
-      <c r="E1915">
-        <v>281.5</v>
+      <c r="D1915" s="2">
+        <v>1912</v>
+      </c>
+      <c r="E1915" s="2">
+        <v>281.22000000000003</v>
       </c>
     </row>
     <row r="1916" spans="1:5" x14ac:dyDescent="0.25">
@@ -27216,11 +27221,11 @@
       <c r="B1916">
         <v>298.57</v>
       </c>
-      <c r="D1916">
-        <v>1914</v>
-      </c>
-      <c r="E1916">
-        <v>281.77</v>
+      <c r="D1916" s="2">
+        <v>1913</v>
+      </c>
+      <c r="E1916" s="2">
+        <v>281.5</v>
       </c>
     </row>
     <row r="1917" spans="1:5" x14ac:dyDescent="0.25">
@@ -27230,11 +27235,11 @@
       <c r="B1917">
         <v>298.88</v>
       </c>
-      <c r="D1917">
-        <v>1915</v>
-      </c>
-      <c r="E1917">
-        <v>282.04000000000002</v>
+      <c r="D1917" s="2">
+        <v>1914</v>
+      </c>
+      <c r="E1917" s="2">
+        <v>281.77999999999997</v>
       </c>
     </row>
     <row r="1918" spans="1:5" x14ac:dyDescent="0.25">
@@ -27244,11 +27249,11 @@
       <c r="B1918">
         <v>299.19</v>
       </c>
-      <c r="D1918">
-        <v>1916</v>
-      </c>
-      <c r="E1918">
-        <v>282.31</v>
+      <c r="D1918" s="2">
+        <v>1915</v>
+      </c>
+      <c r="E1918" s="2">
+        <v>282.06</v>
       </c>
     </row>
     <row r="1919" spans="1:5" x14ac:dyDescent="0.25">
@@ -27258,11 +27263,11 @@
       <c r="B1919">
         <v>299.51</v>
       </c>
-      <c r="D1919">
-        <v>1917</v>
-      </c>
-      <c r="E1919">
-        <v>282.58</v>
+      <c r="D1919" s="2">
+        <v>1916</v>
+      </c>
+      <c r="E1919" s="2">
+        <v>282.33</v>
       </c>
     </row>
     <row r="1920" spans="1:5" x14ac:dyDescent="0.25">
@@ -27272,11 +27277,11 @@
       <c r="B1920">
         <v>299.85000000000002</v>
       </c>
-      <c r="D1920">
-        <v>1918</v>
-      </c>
-      <c r="E1920">
-        <v>282.85000000000002</v>
+      <c r="D1920" s="2">
+        <v>1917</v>
+      </c>
+      <c r="E1920" s="2">
+        <v>282.61</v>
       </c>
     </row>
     <row r="1921" spans="1:5" x14ac:dyDescent="0.25">
@@ -27286,11 +27291,11 @@
       <c r="B1921">
         <v>300.2</v>
       </c>
-      <c r="D1921">
-        <v>1919</v>
-      </c>
-      <c r="E1921">
-        <v>283.12</v>
+      <c r="D1921" s="2">
+        <v>1918</v>
+      </c>
+      <c r="E1921" s="2">
+        <v>282.88</v>
       </c>
     </row>
     <row r="1922" spans="1:5" x14ac:dyDescent="0.25">
@@ -27300,11 +27305,11 @@
       <c r="B1922">
         <v>300.57</v>
       </c>
-      <c r="D1922">
-        <v>1920</v>
-      </c>
-      <c r="E1922">
-        <v>283.38</v>
+      <c r="D1922" s="2">
+        <v>1919</v>
+      </c>
+      <c r="E1922" s="2">
+        <v>283.14999999999998</v>
       </c>
     </row>
     <row r="1923" spans="1:5" x14ac:dyDescent="0.25">
@@ -27314,11 +27319,11 @@
       <c r="B1923">
         <v>300.95</v>
       </c>
-      <c r="D1923">
-        <v>1921</v>
-      </c>
-      <c r="E1923">
-        <v>283.63</v>
+      <c r="D1923" s="2">
+        <v>1920</v>
+      </c>
+      <c r="E1923" s="2">
+        <v>283.41000000000003</v>
       </c>
     </row>
     <row r="1924" spans="1:5" x14ac:dyDescent="0.25">
@@ -27328,11 +27333,11 @@
       <c r="B1924">
         <v>301.35000000000002</v>
       </c>
-      <c r="D1924">
-        <v>1922</v>
-      </c>
-      <c r="E1924">
-        <v>283.88</v>
+      <c r="D1924" s="2">
+        <v>1921</v>
+      </c>
+      <c r="E1924" s="2">
+        <v>283.67</v>
       </c>
     </row>
     <row r="1925" spans="1:5" x14ac:dyDescent="0.25">
@@ -27342,11 +27347,11 @@
       <c r="B1925">
         <v>301.77</v>
       </c>
-      <c r="D1925">
-        <v>1923</v>
-      </c>
-      <c r="E1925">
-        <v>284.13</v>
+      <c r="D1925" s="2">
+        <v>1922</v>
+      </c>
+      <c r="E1925" s="2">
+        <v>283.92</v>
       </c>
     </row>
     <row r="1926" spans="1:5" x14ac:dyDescent="0.25">
@@ -27356,11 +27361,11 @@
       <c r="B1926">
         <v>302.19</v>
       </c>
-      <c r="D1926">
-        <v>1924</v>
-      </c>
-      <c r="E1926">
-        <v>284.37</v>
+      <c r="D1926" s="2">
+        <v>1923</v>
+      </c>
+      <c r="E1926" s="2">
+        <v>284.17</v>
       </c>
     </row>
     <row r="1927" spans="1:5" x14ac:dyDescent="0.25">
@@ -27370,11 +27375,11 @@
       <c r="B1927">
         <v>302.61</v>
       </c>
-      <c r="D1927">
-        <v>1925</v>
-      </c>
-      <c r="E1927">
-        <v>284.61</v>
+      <c r="D1927" s="2">
+        <v>1924</v>
+      </c>
+      <c r="E1927" s="2">
+        <v>284.41000000000003</v>
       </c>
     </row>
     <row r="1928" spans="1:5" x14ac:dyDescent="0.25">
@@ -27384,11 +27389,11 @@
       <c r="B1928">
         <v>303.02</v>
       </c>
-      <c r="D1928">
-        <v>1926</v>
-      </c>
-      <c r="E1928">
-        <v>284.83999999999997</v>
+      <c r="D1928" s="2">
+        <v>1925</v>
+      </c>
+      <c r="E1928" s="2">
+        <v>284.64999999999998</v>
       </c>
     </row>
     <row r="1929" spans="1:5" x14ac:dyDescent="0.25">
@@ -27398,11 +27403,11 @@
       <c r="B1929">
         <v>303.41000000000003</v>
       </c>
-      <c r="D1929">
-        <v>1927</v>
-      </c>
-      <c r="E1929">
-        <v>285.07</v>
+      <c r="D1929" s="2">
+        <v>1926</v>
+      </c>
+      <c r="E1929" s="2">
+        <v>284.88</v>
       </c>
     </row>
     <row r="1930" spans="1:5" x14ac:dyDescent="0.25">
@@ -27412,11 +27417,11 @@
       <c r="B1930">
         <v>303.79000000000002</v>
       </c>
-      <c r="D1930">
-        <v>1928</v>
-      </c>
-      <c r="E1930">
-        <v>285.3</v>
+      <c r="D1930" s="2">
+        <v>1927</v>
+      </c>
+      <c r="E1930" s="2">
+        <v>285.11</v>
       </c>
     </row>
     <row r="1931" spans="1:5" x14ac:dyDescent="0.25">
@@ -27426,11 +27431,11 @@
       <c r="B1931">
         <v>304.14999999999998</v>
       </c>
-      <c r="D1931">
-        <v>1929</v>
-      </c>
-      <c r="E1931">
-        <v>285.52</v>
+      <c r="D1931" s="2">
+        <v>1928</v>
+      </c>
+      <c r="E1931" s="2">
+        <v>285.33999999999997</v>
       </c>
     </row>
     <row r="1932" spans="1:5" x14ac:dyDescent="0.25">
@@ -27440,11 +27445,11 @@
       <c r="B1932">
         <v>304.48</v>
       </c>
-      <c r="D1932">
-        <v>1930</v>
-      </c>
-      <c r="E1932">
-        <v>285.74</v>
+      <c r="D1932" s="2">
+        <v>1929</v>
+      </c>
+      <c r="E1932" s="2">
+        <v>285.56</v>
       </c>
     </row>
     <row r="1933" spans="1:5" x14ac:dyDescent="0.25">
@@ -27454,11 +27459,11 @@
       <c r="B1933">
         <v>304.8</v>
       </c>
-      <c r="D1933">
-        <v>1931</v>
-      </c>
-      <c r="E1933">
-        <v>285.95</v>
+      <c r="D1933" s="2">
+        <v>1930</v>
+      </c>
+      <c r="E1933" s="2">
+        <v>285.77</v>
       </c>
     </row>
     <row r="1934" spans="1:5" x14ac:dyDescent="0.25">
@@ -27468,11 +27473,11 @@
       <c r="B1934">
         <v>305.12</v>
       </c>
-      <c r="D1934">
-        <v>1932</v>
-      </c>
-      <c r="E1934">
-        <v>286.16000000000003</v>
+      <c r="D1934" s="2">
+        <v>1931</v>
+      </c>
+      <c r="E1934" s="2">
+        <v>285.99</v>
       </c>
     </row>
     <row r="1935" spans="1:5" x14ac:dyDescent="0.25">
@@ -27482,11 +27487,11 @@
       <c r="B1935">
         <v>305.42</v>
       </c>
-      <c r="D1935">
-        <v>1933</v>
-      </c>
-      <c r="E1935">
-        <v>286.37</v>
+      <c r="D1935" s="2">
+        <v>1932</v>
+      </c>
+      <c r="E1935" s="2">
+        <v>286.2</v>
       </c>
     </row>
     <row r="1936" spans="1:5" x14ac:dyDescent="0.25">
@@ -27496,11 +27501,11 @@
       <c r="B1936">
         <v>305.73</v>
       </c>
-      <c r="D1936">
-        <v>1934</v>
-      </c>
-      <c r="E1936">
-        <v>286.57</v>
+      <c r="D1936" s="2">
+        <v>1933</v>
+      </c>
+      <c r="E1936" s="2">
+        <v>286.39999999999998</v>
       </c>
     </row>
     <row r="1937" spans="1:5" x14ac:dyDescent="0.25">
@@ -27510,11 +27515,11 @@
       <c r="B1937">
         <v>306.05</v>
       </c>
-      <c r="D1937">
-        <v>1935</v>
-      </c>
-      <c r="E1937">
-        <v>286.77</v>
+      <c r="D1937" s="2">
+        <v>1934</v>
+      </c>
+      <c r="E1937" s="2">
+        <v>286.60000000000002</v>
       </c>
     </row>
     <row r="1938" spans="1:5" x14ac:dyDescent="0.25">
@@ -27524,11 +27529,11 @@
       <c r="B1938">
         <v>306.37</v>
       </c>
-      <c r="D1938">
-        <v>1936</v>
-      </c>
-      <c r="E1938">
-        <v>286.95999999999998</v>
+      <c r="D1938" s="2">
+        <v>1935</v>
+      </c>
+      <c r="E1938" s="2">
+        <v>286.8</v>
       </c>
     </row>
     <row r="1939" spans="1:5" x14ac:dyDescent="0.25">
@@ -27538,11 +27543,11 @@
       <c r="B1939">
         <v>306.70999999999998</v>
       </c>
-      <c r="D1939">
-        <v>1937</v>
-      </c>
-      <c r="E1939">
-        <v>287.14999999999998</v>
+      <c r="D1939" s="2">
+        <v>1936</v>
+      </c>
+      <c r="E1939" s="2">
+        <v>287</v>
       </c>
     </row>
     <row r="1940" spans="1:5" x14ac:dyDescent="0.25">
@@ -27552,11 +27557,11 @@
       <c r="B1940">
         <v>307.07</v>
       </c>
-      <c r="D1940">
-        <v>1938</v>
-      </c>
-      <c r="E1940">
-        <v>287.33999999999997</v>
+      <c r="D1940" s="2">
+        <v>1937</v>
+      </c>
+      <c r="E1940" s="2">
+        <v>287.19</v>
       </c>
     </row>
     <row r="1941" spans="1:5" x14ac:dyDescent="0.25">
@@ -27566,11 +27571,11 @@
       <c r="B1941">
         <v>307.44</v>
       </c>
-      <c r="D1941">
-        <v>1939</v>
-      </c>
-      <c r="E1941">
-        <v>287.52999999999997</v>
+      <c r="D1941" s="2">
+        <v>1938</v>
+      </c>
+      <c r="E1941" s="2">
+        <v>287.38</v>
       </c>
     </row>
     <row r="1942" spans="1:5" x14ac:dyDescent="0.25">
@@ -27580,11 +27585,11 @@
       <c r="B1942">
         <v>307.83999999999997</v>
       </c>
-      <c r="D1942">
-        <v>1940</v>
-      </c>
-      <c r="E1942">
-        <v>287.70999999999998</v>
+      <c r="D1942" s="2">
+        <v>1939</v>
+      </c>
+      <c r="E1942" s="2">
+        <v>287.56</v>
       </c>
     </row>
     <row r="1943" spans="1:5" x14ac:dyDescent="0.25">
@@ -27594,11 +27599,11 @@
       <c r="B1943">
         <v>308.25</v>
       </c>
-      <c r="D1943">
-        <v>1941</v>
-      </c>
-      <c r="E1943">
-        <v>287.89</v>
+      <c r="D1943" s="2">
+        <v>1940</v>
+      </c>
+      <c r="E1943" s="2">
+        <v>287.74</v>
       </c>
     </row>
     <row r="1944" spans="1:5" x14ac:dyDescent="0.25">
@@ -27608,11 +27613,11 @@
       <c r="B1944">
         <v>308.67</v>
       </c>
-      <c r="D1944">
-        <v>1942</v>
-      </c>
-      <c r="E1944">
-        <v>288.07</v>
+      <c r="D1944" s="2">
+        <v>1941</v>
+      </c>
+      <c r="E1944" s="2">
+        <v>287.92</v>
       </c>
     </row>
     <row r="1945" spans="1:5" x14ac:dyDescent="0.25">
@@ -27622,11 +27627,11 @@
       <c r="B1945">
         <v>309.08999999999997</v>
       </c>
-      <c r="D1945">
-        <v>1943</v>
-      </c>
-      <c r="E1945">
-        <v>288.24</v>
+      <c r="D1945" s="2">
+        <v>1942</v>
+      </c>
+      <c r="E1945" s="2">
+        <v>288.10000000000002</v>
       </c>
     </row>
     <row r="1946" spans="1:5" x14ac:dyDescent="0.25">
@@ -27636,11 +27641,11 @@
       <c r="B1946">
         <v>309.49</v>
       </c>
-      <c r="D1946">
-        <v>1944</v>
-      </c>
-      <c r="E1946">
-        <v>288.41000000000003</v>
+      <c r="D1946" s="2">
+        <v>1943</v>
+      </c>
+      <c r="E1946" s="2">
+        <v>288.27</v>
       </c>
     </row>
     <row r="1947" spans="1:5" x14ac:dyDescent="0.25">
@@ -27650,11 +27655,11 @@
       <c r="B1947">
         <v>309.86</v>
       </c>
-      <c r="D1947">
-        <v>1945</v>
-      </c>
-      <c r="E1947">
-        <v>288.58999999999997</v>
+      <c r="D1947" s="2">
+        <v>1944</v>
+      </c>
+      <c r="E1947" s="2">
+        <v>288.44</v>
       </c>
     </row>
     <row r="1948" spans="1:5" x14ac:dyDescent="0.25">
@@ -27664,11 +27669,11 @@
       <c r="B1948">
         <v>310.2</v>
       </c>
-      <c r="D1948">
-        <v>1946</v>
-      </c>
-      <c r="E1948">
-        <v>288.76</v>
+      <c r="D1948" s="2">
+        <v>1945</v>
+      </c>
+      <c r="E1948" s="2">
+        <v>288.61</v>
       </c>
     </row>
     <row r="1949" spans="1:5" x14ac:dyDescent="0.25">
@@ -27678,11 +27683,11 @@
       <c r="B1949">
         <v>310.51</v>
       </c>
-      <c r="D1949">
-        <v>1947</v>
-      </c>
-      <c r="E1949">
-        <v>288.94</v>
+      <c r="D1949" s="2">
+        <v>1946</v>
+      </c>
+      <c r="E1949" s="2">
+        <v>288.77999999999997</v>
       </c>
     </row>
     <row r="1950" spans="1:5" x14ac:dyDescent="0.25">
@@ -27692,11 +27697,11 @@
       <c r="B1950">
         <v>310.79000000000002</v>
       </c>
-      <c r="D1950">
-        <v>1948</v>
-      </c>
-      <c r="E1950">
-        <v>289.12</v>
+      <c r="D1950" s="2">
+        <v>1947</v>
+      </c>
+      <c r="E1950" s="2">
+        <v>288.95999999999998</v>
       </c>
     </row>
     <row r="1951" spans="1:5" x14ac:dyDescent="0.25">
@@ -27706,11 +27711,11 @@
       <c r="B1951">
         <v>311.05</v>
       </c>
-      <c r="D1951">
-        <v>1949</v>
-      </c>
-      <c r="E1951">
-        <v>289.3</v>
+      <c r="D1951" s="2">
+        <v>1948</v>
+      </c>
+      <c r="E1951" s="2">
+        <v>289.13</v>
       </c>
     </row>
     <row r="1952" spans="1:5" x14ac:dyDescent="0.25">
@@ -27720,11 +27725,11 @@
       <c r="B1952">
         <v>311.27999999999997</v>
       </c>
-      <c r="D1952">
-        <v>1950</v>
-      </c>
-      <c r="E1952">
-        <v>289.48</v>
+      <c r="D1952" s="2">
+        <v>1949</v>
+      </c>
+      <c r="E1952" s="2">
+        <v>289.31</v>
       </c>
     </row>
     <row r="1953" spans="1:5" x14ac:dyDescent="0.25">
@@ -27734,11 +27739,11 @@
       <c r="B1953">
         <v>311.51</v>
       </c>
-      <c r="D1953">
-        <v>1951</v>
-      </c>
-      <c r="E1953">
-        <v>289.68</v>
+      <c r="D1953" s="2">
+        <v>1950</v>
+      </c>
+      <c r="E1953" s="2">
+        <v>289.5</v>
       </c>
     </row>
     <row r="1954" spans="1:5" x14ac:dyDescent="0.25">
@@ -27748,11 +27753,11 @@
       <c r="B1954">
         <v>311.72000000000003</v>
       </c>
-      <c r="D1954">
-        <v>1952</v>
-      </c>
-      <c r="E1954">
-        <v>289.87</v>
+      <c r="D1954" s="2">
+        <v>1951</v>
+      </c>
+      <c r="E1954" s="2">
+        <v>289.68</v>
       </c>
     </row>
     <row r="1955" spans="1:5" x14ac:dyDescent="0.25">
@@ -27762,11 +27767,11 @@
       <c r="B1955">
         <v>311.94</v>
       </c>
-      <c r="D1955">
-        <v>1953</v>
-      </c>
-      <c r="E1955">
-        <v>290.07</v>
+      <c r="D1955" s="2">
+        <v>1952</v>
+      </c>
+      <c r="E1955" s="2">
+        <v>289.88</v>
       </c>
     </row>
     <row r="1956" spans="1:5" x14ac:dyDescent="0.25">
@@ -27776,11 +27781,11 @@
       <c r="B1956">
         <v>312.18</v>
       </c>
-      <c r="D1956">
-        <v>1954</v>
-      </c>
-      <c r="E1956">
-        <v>290.27999999999997</v>
+      <c r="D1956" s="2">
+        <v>1953</v>
+      </c>
+      <c r="E1956" s="2">
+        <v>290.08</v>
       </c>
     </row>
     <row r="1957" spans="1:5" x14ac:dyDescent="0.25">
@@ -27790,11 +27795,11 @@
       <c r="B1957">
         <v>312.43</v>
       </c>
-      <c r="D1957">
-        <v>1955</v>
-      </c>
-      <c r="E1957">
-        <v>290.5</v>
+      <c r="D1957" s="2">
+        <v>1954</v>
+      </c>
+      <c r="E1957" s="2">
+        <v>290.29000000000002</v>
       </c>
     </row>
     <row r="1958" spans="1:5" x14ac:dyDescent="0.25">
@@ -27804,11 +27809,11 @@
       <c r="B1958">
         <v>312.70999999999998</v>
       </c>
-      <c r="D1958">
-        <v>1956</v>
-      </c>
-      <c r="E1958">
-        <v>290.72000000000003</v>
+      <c r="D1958" s="2">
+        <v>1955</v>
+      </c>
+      <c r="E1958" s="2">
+        <v>290.5</v>
       </c>
     </row>
     <row r="1959" spans="1:5" x14ac:dyDescent="0.25">
@@ -27818,11 +27823,11 @@
       <c r="B1959">
         <v>313.01</v>
       </c>
-      <c r="D1959">
-        <v>1957</v>
-      </c>
-      <c r="E1959">
-        <v>290.95</v>
+      <c r="D1959" s="2">
+        <v>1956</v>
+      </c>
+      <c r="E1959" s="2">
+        <v>290.72000000000003</v>
       </c>
     </row>
     <row r="1960" spans="1:5" x14ac:dyDescent="0.25">
@@ -27832,11 +27837,11 @@
       <c r="B1960">
         <v>313.33</v>
       </c>
-      <c r="D1960">
-        <v>1958</v>
-      </c>
-      <c r="E1960">
-        <v>291.18</v>
+      <c r="D1960" s="2">
+        <v>1957</v>
+      </c>
+      <c r="E1960" s="2">
+        <v>290.94</v>
       </c>
     </row>
     <row r="1961" spans="1:5" x14ac:dyDescent="0.25">
@@ -27846,11 +27851,11 @@
       <c r="B1961">
         <v>313.67</v>
       </c>
-      <c r="D1961">
-        <v>1959</v>
-      </c>
-      <c r="E1961">
-        <v>291.43</v>
+      <c r="D1961" s="2">
+        <v>1958</v>
+      </c>
+      <c r="E1961" s="2">
+        <v>291.18</v>
       </c>
     </row>
     <row r="1962" spans="1:5" x14ac:dyDescent="0.25">
@@ -27860,11 +27865,11 @@
       <c r="B1962">
         <v>314.04000000000002</v>
       </c>
-      <c r="D1962">
-        <v>1960</v>
-      </c>
-      <c r="E1962">
-        <v>291.69</v>
+      <c r="D1962" s="2">
+        <v>1959</v>
+      </c>
+      <c r="E1962" s="2">
+        <v>291.42</v>
       </c>
     </row>
     <row r="1963" spans="1:5" x14ac:dyDescent="0.25">
@@ -27874,11 +27879,11 @@
       <c r="B1963">
         <v>314.43</v>
       </c>
-      <c r="D1963">
-        <v>1961</v>
-      </c>
-      <c r="E1963">
-        <v>291.95</v>
+      <c r="D1963" s="2">
+        <v>1960</v>
+      </c>
+      <c r="E1963" s="2">
+        <v>291.67</v>
       </c>
     </row>
     <row r="1964" spans="1:5" x14ac:dyDescent="0.25">
@@ -27888,11 +27893,11 @@
       <c r="B1964">
         <v>314.83999999999997</v>
       </c>
-      <c r="D1964">
-        <v>1962</v>
-      </c>
-      <c r="E1964">
-        <v>292.24</v>
+      <c r="D1964" s="2">
+        <v>1961</v>
+      </c>
+      <c r="E1964" s="2">
+        <v>291.93</v>
       </c>
     </row>
     <row r="1965" spans="1:5" x14ac:dyDescent="0.25">
@@ -27902,11 +27907,11 @@
       <c r="B1965">
         <v>315.27999999999997</v>
       </c>
-      <c r="D1965">
-        <v>1963</v>
-      </c>
-      <c r="E1965">
-        <v>292.52999999999997</v>
+      <c r="D1965" s="2">
+        <v>1962</v>
+      </c>
+      <c r="E1965" s="2">
+        <v>292.20999999999998</v>
       </c>
     </row>
     <row r="1966" spans="1:5" x14ac:dyDescent="0.25">
@@ -27916,11 +27921,11 @@
       <c r="B1966">
         <v>315.74</v>
       </c>
-      <c r="D1966">
-        <v>1964</v>
-      </c>
-      <c r="E1966">
-        <v>292.83999999999997</v>
+      <c r="D1966" s="2">
+        <v>1963</v>
+      </c>
+      <c r="E1966" s="2">
+        <v>292.5</v>
       </c>
     </row>
     <row r="1967" spans="1:5" x14ac:dyDescent="0.25">
@@ -27930,11 +27935,11 @@
       <c r="B1967">
         <v>316.26</v>
       </c>
-      <c r="D1967">
-        <v>1965</v>
-      </c>
-      <c r="E1967">
-        <v>293.16000000000003</v>
+      <c r="D1967" s="2">
+        <v>1964</v>
+      </c>
+      <c r="E1967" s="2">
+        <v>292.81</v>
       </c>
     </row>
     <row r="1968" spans="1:5" x14ac:dyDescent="0.25">
@@ -27944,11 +27949,11 @@
       <c r="B1968">
         <v>316.82</v>
       </c>
-      <c r="D1968">
-        <v>1966</v>
-      </c>
-      <c r="E1968">
-        <v>293.5</v>
+      <c r="D1968" s="2">
+        <v>1965</v>
+      </c>
+      <c r="E1968" s="2">
+        <v>293.13</v>
       </c>
     </row>
     <row r="1969" spans="1:5" x14ac:dyDescent="0.25">
@@ -27958,11 +27963,11 @@
       <c r="B1969">
         <v>317.44</v>
       </c>
-      <c r="D1969">
-        <v>1967</v>
-      </c>
-      <c r="E1969">
-        <v>293.86</v>
+      <c r="D1969" s="2">
+        <v>1966</v>
+      </c>
+      <c r="E1969" s="2">
+        <v>293.45999999999998</v>
       </c>
     </row>
     <row r="1970" spans="1:5" x14ac:dyDescent="0.25">
@@ -27972,11 +27977,11 @@
       <c r="B1970">
         <v>318.12</v>
       </c>
-      <c r="D1970">
-        <v>1968</v>
-      </c>
-      <c r="E1970">
-        <v>294.23</v>
+      <c r="D1970" s="2">
+        <v>1967</v>
+      </c>
+      <c r="E1970" s="2">
+        <v>293.82</v>
       </c>
     </row>
     <row r="1971" spans="1:5" x14ac:dyDescent="0.25">
@@ -27986,11 +27991,11 @@
       <c r="B1971">
         <v>318.86</v>
       </c>
-      <c r="D1971">
-        <v>1969</v>
-      </c>
-      <c r="E1971">
-        <v>294.63</v>
+      <c r="D1971" s="2">
+        <v>1968</v>
+      </c>
+      <c r="E1971" s="2">
+        <v>294.19</v>
       </c>
     </row>
     <row r="1972" spans="1:5" x14ac:dyDescent="0.25">
@@ -28000,11 +28005,11 @@
       <c r="B1972">
         <v>319.64999999999998</v>
       </c>
-      <c r="D1972">
-        <v>1970</v>
-      </c>
-      <c r="E1972">
-        <v>295.04000000000002</v>
+      <c r="D1972" s="2">
+        <v>1969</v>
+      </c>
+      <c r="E1972" s="2">
+        <v>294.58999999999997</v>
       </c>
     </row>
     <row r="1973" spans="1:5" x14ac:dyDescent="0.25">
@@ -28014,11 +28019,11 @@
       <c r="B1973">
         <v>320.49</v>
       </c>
-      <c r="D1973">
-        <v>1971</v>
-      </c>
-      <c r="E1973">
-        <v>295.48</v>
+      <c r="D1973" s="2">
+        <v>1970</v>
+      </c>
+      <c r="E1973" s="2">
+        <v>295</v>
       </c>
     </row>
     <row r="1974" spans="1:5" x14ac:dyDescent="0.25">
@@ -28028,11 +28033,11 @@
       <c r="B1974">
         <v>321.39</v>
       </c>
-      <c r="D1974">
-        <v>1972</v>
-      </c>
-      <c r="E1974">
-        <v>295.93</v>
+      <c r="D1974" s="2">
+        <v>1971</v>
+      </c>
+      <c r="E1974" s="2">
+        <v>295.44</v>
       </c>
     </row>
     <row r="1975" spans="1:5" x14ac:dyDescent="0.25">
@@ -28042,11 +28047,11 @@
       <c r="B1975">
         <v>322.35000000000002</v>
       </c>
-      <c r="D1975">
-        <v>1973</v>
-      </c>
-      <c r="E1975">
-        <v>296.39999999999998</v>
+      <c r="D1975" s="2">
+        <v>1972</v>
+      </c>
+      <c r="E1975" s="2">
+        <v>295.89</v>
       </c>
     </row>
     <row r="1976" spans="1:5" x14ac:dyDescent="0.25">
@@ -28056,11 +28061,11 @@
       <c r="B1976">
         <v>323.35000000000002</v>
       </c>
-      <c r="D1976">
-        <v>1974</v>
-      </c>
-      <c r="E1976">
-        <v>296.89</v>
+      <c r="D1976" s="2">
+        <v>1973</v>
+      </c>
+      <c r="E1976" s="2">
+        <v>296.37</v>
       </c>
     </row>
     <row r="1977" spans="1:5" x14ac:dyDescent="0.25">
@@ -28070,11 +28075,11 @@
       <c r="B1977">
         <v>324.39999999999998</v>
       </c>
-      <c r="D1977">
-        <v>1975</v>
-      </c>
-      <c r="E1977">
-        <v>297.39999999999998</v>
+      <c r="D1977" s="2">
+        <v>1974</v>
+      </c>
+      <c r="E1977" s="2">
+        <v>296.86</v>
       </c>
     </row>
     <row r="1978" spans="1:5" x14ac:dyDescent="0.25">
@@ -28084,11 +28089,11 @@
       <c r="B1978">
         <v>325.48</v>
       </c>
-      <c r="D1978">
-        <v>1976</v>
-      </c>
-      <c r="E1978">
-        <v>297.93</v>
+      <c r="D1978" s="2">
+        <v>1975</v>
+      </c>
+      <c r="E1978" s="2">
+        <v>297.38</v>
       </c>
     </row>
     <row r="1979" spans="1:5" x14ac:dyDescent="0.25">
@@ -28098,11 +28103,11 @@
       <c r="B1979">
         <v>326.60000000000002</v>
       </c>
-      <c r="D1979">
-        <v>1977</v>
-      </c>
-      <c r="E1979">
-        <v>298.47000000000003</v>
+      <c r="D1979" s="2">
+        <v>1976</v>
+      </c>
+      <c r="E1979" s="2">
+        <v>297.91000000000003</v>
       </c>
     </row>
     <row r="1980" spans="1:5" x14ac:dyDescent="0.25">
@@ -28112,11 +28117,11 @@
       <c r="B1980">
         <v>327.75</v>
       </c>
-      <c r="D1980">
-        <v>1978</v>
-      </c>
-      <c r="E1980">
-        <v>299.02999999999997</v>
+      <c r="D1980" s="2">
+        <v>1977</v>
+      </c>
+      <c r="E1980" s="2">
+        <v>298.45</v>
       </c>
     </row>
     <row r="1981" spans="1:5" x14ac:dyDescent="0.25">
@@ -28126,11 +28131,11 @@
       <c r="B1981">
         <v>328.93</v>
       </c>
-      <c r="D1981">
-        <v>1979</v>
-      </c>
-      <c r="E1981">
-        <v>299.60000000000002</v>
+      <c r="D1981" s="2">
+        <v>1978</v>
+      </c>
+      <c r="E1981" s="2">
+        <v>299.01</v>
       </c>
     </row>
     <row r="1982" spans="1:5" x14ac:dyDescent="0.25">
@@ -28140,11 +28145,11 @@
       <c r="B1982">
         <v>330.12</v>
       </c>
-      <c r="D1982">
-        <v>1980</v>
-      </c>
-      <c r="E1982">
-        <v>300.19</v>
+      <c r="D1982" s="2">
+        <v>1979</v>
+      </c>
+      <c r="E1982" s="2">
+        <v>299.58999999999997</v>
       </c>
     </row>
     <row r="1983" spans="1:5" x14ac:dyDescent="0.25">
@@ -28154,11 +28159,11 @@
       <c r="B1983">
         <v>331.33</v>
       </c>
-      <c r="D1983">
-        <v>1981</v>
-      </c>
-      <c r="E1983">
-        <v>300.79000000000002</v>
+      <c r="D1983" s="2">
+        <v>1980</v>
+      </c>
+      <c r="E1983" s="2">
+        <v>300.18</v>
       </c>
     </row>
     <row r="1984" spans="1:5" x14ac:dyDescent="0.25">
@@ -28168,11 +28173,11 @@
       <c r="B1984">
         <v>332.56</v>
       </c>
-      <c r="D1984">
-        <v>1982</v>
-      </c>
-      <c r="E1984">
-        <v>301.39999999999998</v>
+      <c r="D1984" s="2">
+        <v>1981</v>
+      </c>
+      <c r="E1984" s="2">
+        <v>300.77999999999997</v>
       </c>
     </row>
     <row r="1985" spans="1:5" x14ac:dyDescent="0.25">
@@ -28182,11 +28187,11 @@
       <c r="B1985">
         <v>333.8</v>
       </c>
-      <c r="D1985">
-        <v>1983</v>
-      </c>
-      <c r="E1985">
-        <v>302.02999999999997</v>
+      <c r="D1985" s="2">
+        <v>1982</v>
+      </c>
+      <c r="E1985" s="2">
+        <v>301.39</v>
       </c>
     </row>
     <row r="1986" spans="1:5" x14ac:dyDescent="0.25">
@@ -28196,11 +28201,11 @@
       <c r="B1986">
         <v>335.06</v>
       </c>
-      <c r="D1986">
-        <v>1984</v>
-      </c>
-      <c r="E1986">
-        <v>302.66000000000003</v>
+      <c r="D1986" s="2">
+        <v>1983</v>
+      </c>
+      <c r="E1986" s="2">
+        <v>302.02</v>
       </c>
     </row>
     <row r="1987" spans="1:5" x14ac:dyDescent="0.25">
@@ -28210,11 +28215,11 @@
       <c r="B1987">
         <v>336.35</v>
       </c>
-      <c r="D1987">
-        <v>1985</v>
-      </c>
-      <c r="E1987">
-        <v>303.31</v>
+      <c r="D1987" s="2">
+        <v>1984</v>
+      </c>
+      <c r="E1987" s="2">
+        <v>302.64999999999998</v>
       </c>
     </row>
     <row r="1988" spans="1:5" x14ac:dyDescent="0.25">
@@ -28224,11 +28229,11 @@
       <c r="B1988">
         <v>337.65</v>
       </c>
-      <c r="D1988">
-        <v>1986</v>
-      </c>
-      <c r="E1988">
-        <v>303.98</v>
+      <c r="D1988" s="2">
+        <v>1985</v>
+      </c>
+      <c r="E1988" s="2">
+        <v>303.31</v>
       </c>
     </row>
     <row r="1989" spans="1:5" x14ac:dyDescent="0.25">
@@ -28238,11 +28243,11 @@
       <c r="B1989">
         <v>338.98</v>
       </c>
-      <c r="D1989">
-        <v>1987</v>
-      </c>
-      <c r="E1989">
-        <v>304.64999999999998</v>
+      <c r="D1989" s="2">
+        <v>1986</v>
+      </c>
+      <c r="E1989" s="2">
+        <v>303.97000000000003</v>
       </c>
     </row>
     <row r="1990" spans="1:5" x14ac:dyDescent="0.25">
@@ -28252,11 +28257,11 @@
       <c r="B1990">
         <v>340.32</v>
       </c>
-      <c r="D1990">
-        <v>1988</v>
-      </c>
-      <c r="E1990">
-        <v>305.33999999999997</v>
+      <c r="D1990" s="2">
+        <v>1987</v>
+      </c>
+      <c r="E1990" s="2">
+        <v>304.64999999999998</v>
       </c>
     </row>
     <row r="1991" spans="1:5" x14ac:dyDescent="0.25">
@@ -28266,11 +28271,11 @@
       <c r="B1991">
         <v>341.69</v>
       </c>
-      <c r="D1991">
-        <v>1989</v>
-      </c>
-      <c r="E1991">
-        <v>306.04000000000002</v>
+      <c r="D1991" s="2">
+        <v>1988</v>
+      </c>
+      <c r="E1991" s="2">
+        <v>305.33999999999997</v>
       </c>
     </row>
     <row r="1992" spans="1:5" x14ac:dyDescent="0.25">
@@ -28280,11 +28285,11 @@
       <c r="B1992">
         <v>343.09</v>
       </c>
-      <c r="D1992">
-        <v>1990</v>
-      </c>
-      <c r="E1992">
-        <v>306.75</v>
+      <c r="D1992" s="2">
+        <v>1989</v>
+      </c>
+      <c r="E1992" s="2">
+        <v>306.04000000000002</v>
       </c>
     </row>
     <row r="1993" spans="1:5" x14ac:dyDescent="0.25">
@@ -28294,11 +28299,11 @@
       <c r="B1993">
         <v>344.51</v>
       </c>
-      <c r="D1993">
-        <v>1991</v>
-      </c>
-      <c r="E1993">
-        <v>307.45999999999998</v>
+      <c r="D1993" s="2">
+        <v>1990</v>
+      </c>
+      <c r="E1993" s="2">
+        <v>306.75</v>
       </c>
     </row>
     <row r="1994" spans="1:5" x14ac:dyDescent="0.25">
@@ -28308,11 +28313,11 @@
       <c r="B1994">
         <v>345.96</v>
       </c>
-      <c r="D1994">
-        <v>1992</v>
-      </c>
-      <c r="E1994">
-        <v>308.18</v>
+      <c r="D1994" s="2">
+        <v>1991</v>
+      </c>
+      <c r="E1994" s="2">
+        <v>307.45999999999998</v>
       </c>
     </row>
     <row r="1995" spans="1:5" x14ac:dyDescent="0.25">
@@ -28322,11 +28327,11 @@
       <c r="B1995">
         <v>347.43</v>
       </c>
-      <c r="D1995">
-        <v>1993</v>
-      </c>
-      <c r="E1995">
-        <v>308.91000000000003</v>
+      <c r="D1995" s="2">
+        <v>1992</v>
+      </c>
+      <c r="E1995" s="2">
+        <v>308.18</v>
       </c>
     </row>
     <row r="1996" spans="1:5" x14ac:dyDescent="0.25">
@@ -28336,11 +28341,11 @@
       <c r="B1996">
         <v>348.91</v>
       </c>
-      <c r="D1996">
-        <v>1994</v>
-      </c>
-      <c r="E1996">
-        <v>309.64</v>
+      <c r="D1996" s="2">
+        <v>1993</v>
+      </c>
+      <c r="E1996" s="2">
+        <v>308.91000000000003</v>
       </c>
     </row>
     <row r="1997" spans="1:5" x14ac:dyDescent="0.25">
@@ -28350,11 +28355,11 @@
       <c r="B1997">
         <v>350.38</v>
       </c>
-      <c r="D1997">
-        <v>1995</v>
-      </c>
-      <c r="E1997">
-        <v>310.37</v>
+      <c r="D1997" s="2">
+        <v>1994</v>
+      </c>
+      <c r="E1997" s="2">
+        <v>309.64</v>
       </c>
     </row>
     <row r="1998" spans="1:5" x14ac:dyDescent="0.25">
@@ -28364,11 +28369,11 @@
       <c r="B1998">
         <v>351.84</v>
       </c>
-      <c r="D1998">
-        <v>1996</v>
-      </c>
-      <c r="E1998">
-        <v>311.12</v>
+      <c r="D1998" s="2">
+        <v>1995</v>
+      </c>
+      <c r="E1998" s="2">
+        <v>310.37</v>
       </c>
     </row>
     <row r="1999" spans="1:5" x14ac:dyDescent="0.25">
@@ -28378,11 +28383,11 @@
       <c r="B1999">
         <v>353.27</v>
       </c>
-      <c r="D1999">
-        <v>1997</v>
-      </c>
-      <c r="E1999">
-        <v>311.87</v>
+      <c r="D1999" s="2">
+        <v>1996</v>
+      </c>
+      <c r="E1999" s="2">
+        <v>311.12</v>
       </c>
     </row>
     <row r="2000" spans="1:5" x14ac:dyDescent="0.25">
@@ -28392,11 +28397,11 @@
       <c r="B2000">
         <v>354.67</v>
       </c>
-      <c r="D2000">
-        <v>1998</v>
-      </c>
-      <c r="E2000">
-        <v>312.63</v>
+      <c r="D2000" s="2">
+        <v>1997</v>
+      </c>
+      <c r="E2000" s="2">
+        <v>311.88</v>
       </c>
     </row>
     <row r="2001" spans="1:5" x14ac:dyDescent="0.25">
@@ -28406,11 +28411,11 @@
       <c r="B2001">
         <v>356.1</v>
       </c>
-      <c r="D2001">
-        <v>1999</v>
-      </c>
-      <c r="E2001">
-        <v>313.39</v>
+      <c r="D2001" s="2">
+        <v>1998</v>
+      </c>
+      <c r="E2001" s="2">
+        <v>312.64</v>
       </c>
     </row>
     <row r="2002" spans="1:5" x14ac:dyDescent="0.25">
@@ -28420,11 +28425,11 @@
       <c r="B2002">
         <v>357.6</v>
       </c>
-      <c r="D2002">
-        <v>2000</v>
-      </c>
-      <c r="E2002">
-        <v>314.14999999999998</v>
+      <c r="D2002" s="2">
+        <v>1999</v>
+      </c>
+      <c r="E2002" s="2">
+        <v>313.39999999999998</v>
       </c>
     </row>
     <row r="2003" spans="1:5" x14ac:dyDescent="0.25">
@@ -28434,11 +28439,11 @@
       <c r="B2003">
         <v>359.19</v>
       </c>
-      <c r="D2003">
-        <v>2001</v>
-      </c>
-      <c r="E2003">
-        <v>314.89999999999998</v>
+      <c r="D2003" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E2003" s="2">
+        <v>314.16000000000003</v>
       </c>
     </row>
     <row r="2004" spans="1:5" x14ac:dyDescent="0.25">
@@ -28448,11 +28453,11 @@
       <c r="B2004">
         <v>360.85</v>
       </c>
-      <c r="D2004">
-        <v>2002</v>
-      </c>
-      <c r="E2004">
-        <v>315.64999999999998</v>
+      <c r="D2004" s="2">
+        <v>2001</v>
+      </c>
+      <c r="E2004" s="2">
+        <v>314.92</v>
       </c>
     </row>
     <row r="2005" spans="1:5" x14ac:dyDescent="0.25">
@@ -28462,11 +28467,11 @@
       <c r="B2005">
         <v>362.61</v>
       </c>
-      <c r="D2005">
-        <v>2003</v>
-      </c>
-      <c r="E2005">
-        <v>316.39999999999998</v>
+      <c r="D2005" s="2">
+        <v>2002</v>
+      </c>
+      <c r="E2005" s="2">
+        <v>315.66000000000003</v>
       </c>
     </row>
     <row r="2006" spans="1:5" x14ac:dyDescent="0.25">
@@ -28476,11 +28481,11 @@
       <c r="B2006">
         <v>364.43</v>
       </c>
-      <c r="D2006">
-        <v>2004</v>
-      </c>
-      <c r="E2006">
-        <v>317.14999999999998</v>
+      <c r="D2006" s="2">
+        <v>2003</v>
+      </c>
+      <c r="E2006" s="2">
+        <v>316.39999999999998</v>
       </c>
     </row>
     <row r="2007" spans="1:5" x14ac:dyDescent="0.25">
@@ -28490,11 +28495,11 @@
       <c r="B2007">
         <v>366.25</v>
       </c>
-      <c r="D2007">
-        <v>2005</v>
-      </c>
-      <c r="E2007">
-        <v>317.92</v>
+      <c r="D2007" s="2">
+        <v>2004</v>
+      </c>
+      <c r="E2007" s="2">
+        <v>317.14999999999998</v>
       </c>
     </row>
     <row r="2008" spans="1:5" x14ac:dyDescent="0.25">
@@ -28504,11 +28509,11 @@
       <c r="B2008">
         <v>368.08</v>
       </c>
-      <c r="D2008">
-        <v>2006</v>
-      </c>
-      <c r="E2008">
-        <v>318.7</v>
+      <c r="D2008" s="2">
+        <v>2005</v>
+      </c>
+      <c r="E2008" s="2">
+        <v>317.91000000000003</v>
       </c>
     </row>
     <row r="2009" spans="1:5" x14ac:dyDescent="0.25">
@@ -28518,11 +28523,11 @@
       <c r="B2009">
         <v>369.95</v>
       </c>
-      <c r="D2009">
-        <v>2007</v>
-      </c>
-      <c r="E2009">
-        <v>319.49</v>
+      <c r="D2009" s="2">
+        <v>2006</v>
+      </c>
+      <c r="E2009" s="2">
+        <v>318.69</v>
       </c>
     </row>
     <row r="2010" spans="1:5" x14ac:dyDescent="0.25">
@@ -28532,11 +28537,11 @@
       <c r="B2010">
         <v>371.87</v>
       </c>
-      <c r="D2010">
-        <v>2008</v>
-      </c>
-      <c r="E2010">
-        <v>320.31</v>
+      <c r="D2010" s="2">
+        <v>2007</v>
+      </c>
+      <c r="E2010" s="2">
+        <v>319.48</v>
       </c>
     </row>
     <row r="2011" spans="1:5" x14ac:dyDescent="0.25">
@@ -28546,11 +28551,11 @@
       <c r="B2011">
         <v>373.83</v>
       </c>
-      <c r="D2011">
-        <v>2009</v>
-      </c>
-      <c r="E2011">
-        <v>321.14999999999998</v>
+      <c r="D2011" s="2">
+        <v>2008</v>
+      </c>
+      <c r="E2011" s="2">
+        <v>320.3</v>
       </c>
     </row>
     <row r="2012" spans="1:5" x14ac:dyDescent="0.25">
@@ -28560,11 +28565,11 @@
       <c r="B2012">
         <v>375.78</v>
       </c>
-      <c r="D2012">
-        <v>2010</v>
-      </c>
-      <c r="E2012">
-        <v>322</v>
+      <c r="D2012" s="2">
+        <v>2009</v>
+      </c>
+      <c r="E2012" s="2">
+        <v>321.13</v>
       </c>
     </row>
     <row r="2013" spans="1:5" x14ac:dyDescent="0.25">
@@ -28574,11 +28579,11 @@
       <c r="B2013">
         <v>377.72</v>
       </c>
-      <c r="D2013">
-        <v>2011</v>
-      </c>
-      <c r="E2013">
-        <v>322.88</v>
+      <c r="D2013" s="2">
+        <v>2010</v>
+      </c>
+      <c r="E2013" s="2">
+        <v>321.99</v>
       </c>
     </row>
     <row r="2014" spans="1:5" x14ac:dyDescent="0.25">
@@ -28588,11 +28593,11 @@
       <c r="B2014">
         <v>379.66</v>
       </c>
-      <c r="D2014">
-        <v>2012</v>
-      </c>
-      <c r="E2014">
-        <v>323.77999999999997</v>
+      <c r="D2014" s="2">
+        <v>2011</v>
+      </c>
+      <c r="E2014" s="2">
+        <v>322.87</v>
       </c>
     </row>
     <row r="2015" spans="1:5" x14ac:dyDescent="0.25">
@@ -28602,11 +28607,11 @@
       <c r="B2015">
         <v>381.58</v>
       </c>
-      <c r="D2015">
-        <v>2013</v>
-      </c>
-      <c r="E2015">
-        <v>324.7</v>
+      <c r="D2015" s="2">
+        <v>2012</v>
+      </c>
+      <c r="E2015" s="2">
+        <v>323.77</v>
       </c>
     </row>
     <row r="2016" spans="1:5" x14ac:dyDescent="0.25">
@@ -28616,11 +28621,11 @@
       <c r="B2016">
         <v>383.5</v>
       </c>
-      <c r="D2016">
-        <v>2014</v>
-      </c>
-      <c r="E2016">
-        <v>325.64</v>
+      <c r="D2016" s="2">
+        <v>2013</v>
+      </c>
+      <c r="E2016" s="2">
+        <v>324.69</v>
       </c>
     </row>
     <row r="2017" spans="1:5" x14ac:dyDescent="0.25">
@@ -28630,11 +28635,11 @@
       <c r="B2017">
         <v>385.44</v>
       </c>
-      <c r="D2017">
-        <v>2015</v>
-      </c>
-      <c r="E2017">
-        <v>326.61</v>
+      <c r="D2017" s="2">
+        <v>2014</v>
+      </c>
+      <c r="E2017" s="2">
+        <v>325.63</v>
       </c>
     </row>
     <row r="2018" spans="1:5" x14ac:dyDescent="0.25">
@@ -28644,11 +28649,11 @@
       <c r="B2018">
         <v>387.44</v>
       </c>
-      <c r="D2018">
-        <v>2016</v>
-      </c>
-      <c r="E2018">
-        <v>327.58999999999997</v>
+      <c r="D2018" s="2">
+        <v>2015</v>
+      </c>
+      <c r="E2018" s="2">
+        <v>326.58999999999997</v>
       </c>
     </row>
     <row r="2019" spans="1:5" x14ac:dyDescent="0.25">
@@ -28658,11 +28663,11 @@
       <c r="B2019">
         <v>389.53</v>
       </c>
-      <c r="D2019">
-        <v>2017</v>
-      </c>
-      <c r="E2019">
-        <v>328.6</v>
+      <c r="D2019" s="2">
+        <v>2016</v>
+      </c>
+      <c r="E2019" s="2">
+        <v>327.57</v>
       </c>
     </row>
     <row r="2020" spans="1:5" x14ac:dyDescent="0.25">
@@ -28672,11 +28677,11 @@
       <c r="B2020">
         <v>391.73</v>
       </c>
-      <c r="D2020">
-        <v>2018</v>
-      </c>
-      <c r="E2020">
-        <v>329.63</v>
+      <c r="D2020" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E2020" s="2">
+        <v>328.58</v>
       </c>
     </row>
     <row r="2021" spans="1:5" x14ac:dyDescent="0.25">
@@ -28686,11 +28691,11 @@
       <c r="B2021">
         <v>394.02</v>
       </c>
-      <c r="D2021">
-        <v>2019</v>
-      </c>
-      <c r="E2021">
-        <v>330.68</v>
+      <c r="D2021" s="2">
+        <v>2018</v>
+      </c>
+      <c r="E2021" s="2">
+        <v>329.61</v>
       </c>
     </row>
     <row r="2022" spans="1:5" x14ac:dyDescent="0.25">
@@ -28700,11 +28705,11 @@
       <c r="B2022">
         <v>396.4</v>
       </c>
-      <c r="D2022">
-        <v>2020</v>
-      </c>
-      <c r="E2022">
-        <v>331.76</v>
+      <c r="D2022" s="2">
+        <v>2019</v>
+      </c>
+      <c r="E2022" s="2">
+        <v>330.67</v>
       </c>
     </row>
     <row r="2023" spans="1:5" x14ac:dyDescent="0.25">
@@ -28714,11 +28719,11 @@
       <c r="B2023">
         <v>398.83</v>
       </c>
-      <c r="D2023">
-        <v>2021</v>
-      </c>
-      <c r="E2023">
-        <v>332.86</v>
+      <c r="D2023" s="2">
+        <v>2020</v>
+      </c>
+      <c r="E2023" s="2">
+        <v>331.75</v>
       </c>
     </row>
     <row r="2024" spans="1:5" x14ac:dyDescent="0.25">
@@ -28728,11 +28733,11 @@
       <c r="B2024">
         <v>401.29</v>
       </c>
-      <c r="D2024">
-        <v>2022</v>
-      </c>
-      <c r="E2024">
-        <v>333.97</v>
+      <c r="D2024" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E2024" s="2">
+        <v>332.86</v>
       </c>
     </row>
     <row r="2025" spans="1:5" x14ac:dyDescent="0.25">
@@ -28742,11 +28747,11 @@
       <c r="B2025">
         <v>403.73</v>
       </c>
-      <c r="D2025">
-        <v>2023</v>
-      </c>
-      <c r="E2025">
-        <v>335.1</v>
+      <c r="D2025" s="2">
+        <v>2022</v>
+      </c>
+      <c r="E2025" s="2">
+        <v>333.99</v>
       </c>
     </row>
     <row r="2026" spans="1:5" x14ac:dyDescent="0.25">
@@ -28756,11 +28761,11 @@
       <c r="B2026">
         <v>406.15</v>
       </c>
-      <c r="D2026">
-        <v>2024</v>
-      </c>
-      <c r="E2026">
-        <v>336.23</v>
+      <c r="D2026" s="2">
+        <v>2023</v>
+      </c>
+      <c r="E2026" s="2">
+        <v>335.12</v>
       </c>
     </row>
     <row r="2027" spans="1:5" x14ac:dyDescent="0.25">
@@ -28770,11 +28775,11 @@
       <c r="B2027">
         <v>408.56</v>
       </c>
-      <c r="D2027">
-        <v>2025</v>
-      </c>
-      <c r="E2027">
-        <v>337.36</v>
+      <c r="D2027" s="2">
+        <v>2024</v>
+      </c>
+      <c r="E2027" s="2">
+        <v>336.26</v>
       </c>
     </row>
     <row r="2028" spans="1:5" x14ac:dyDescent="0.25">
@@ -28783,6 +28788,12 @@
       </c>
       <c r="B2028">
         <v>410.97</v>
+      </c>
+      <c r="D2028" s="2">
+        <v>2025</v>
+      </c>
+      <c r="E2028" s="2">
+        <v>337.41</v>
       </c>
     </row>
     <row r="2029" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>